<commit_message>
Formula Excel Template Updated
Formula Excel Template Updated
</commit_message>
<xml_diff>
--- a/Formula Excel Template.xlsx
+++ b/Formula Excel Template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEE5DA8A-F772-4B0E-A554-1053E2C64027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Max-Min" sheetId="9" r:id="rId1"/>
@@ -25,9 +19,9 @@
     <sheet name="Concatenate" sheetId="1" r:id="rId10"/>
     <sheet name="Days-NetworkDays" sheetId="13" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -44,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="90">
   <si>
     <t>FirstName</t>
   </si>
@@ -286,12 +280,6 @@
     <t>COUNTIFS</t>
   </si>
   <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
     <t>IF</t>
   </si>
   <si>
@@ -308,13 +296,25 @@
   </si>
   <si>
     <t>Right</t>
+  </si>
+  <si>
+    <t>Max Age</t>
+  </si>
+  <si>
+    <t>Min Age</t>
+  </si>
+  <si>
+    <t>Max StartDate</t>
+  </si>
+  <si>
+    <t>MinStartDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,12 +329,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -349,11 +355,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +424,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -466,7 +476,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -660,30 +670,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80D7546-D251-4908-B99A-2A3B4BFE22EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -711,14 +722,8 @@
       <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -749,7 +754,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -780,7 +785,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -809,7 +814,7 @@
         <v>42986</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -838,7 +843,7 @@
         <v>42341</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -867,7 +872,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -896,7 +901,7 @@
         <v>41528</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -925,7 +930,7 @@
         <v>41551</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -954,7 +959,7 @@
         <v>42116</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -981,6 +986,42 @@
       </c>
       <c r="I10" s="1">
         <v>40800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="D11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11">
+        <f>MAX(D2:D10)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="D12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12">
+        <f>MIN(D2:D14)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="D13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="1">
+        <f>MAX(H2:H10)</f>
+        <v>37933</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="D14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="1">
+        <f>MIN(H2:H10)</f>
+        <v>35040</v>
       </c>
     </row>
   </sheetData>
@@ -989,17 +1030,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB977C31-5FD1-4473-A6A1-29ABAD3F7755}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="10.44140625" customWidth="1"/>
     <col min="3" max="5" width="10.6640625" customWidth="1"/>
@@ -1009,7 +1050,7 @@
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1037,11 +1078,11 @@
       <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1069,8 +1110,12 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J2" t="str">
+        <f>CONCATENATE(B2," ",C2)</f>
+        <v>Jim Halpert</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1098,8 +1143,12 @@
       <c r="I3" s="1">
         <v>42287</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">CONCATENATE(B3," ",C3)</f>
+        <v>Pam Beasley</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1127,8 +1176,12 @@
       <c r="I4" s="1">
         <v>42986</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Dwight Schrute</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1156,8 +1209,12 @@
       <c r="I5" s="1">
         <v>42341</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Angela Martin</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1185,8 +1242,12 @@
       <c r="I6" s="1">
         <v>42977</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Toby Flenderson</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1214,8 +1275,12 @@
       <c r="I7" s="1">
         <v>41528</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Michael Scott</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1243,8 +1308,12 @@
       <c r="I8" s="1">
         <v>41551</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Meredith Palmer</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1272,8 +1341,12 @@
       <c r="I9" s="1">
         <v>42116</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Stanley Hudson</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1301,16 +1374,20 @@
       <c r="I10" s="1">
         <v>40800</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Kevin Malone</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="H11" t="str">
-        <f t="shared" ref="H3:H12" si="0">CONCATENATE(B11," ",C11)</f>
+        <f t="shared" ref="H11:H12" si="1">CONCATENATE(B11," ",C11)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -1320,342 +1397,350 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137ACEFD-E950-4ACE-A7FD-83ED10CB531A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45000</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2">
+        <f>DAYS360(H2,I2)</f>
+        <v>5158</v>
+      </c>
+      <c r="K2">
+        <f>NETWORKDAYS(H2,I2)</f>
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2">
+        <v>36000</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2">
+        <v>63000</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2">
+        <v>47000</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2">
+        <v>50000</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2">
+        <v>65000</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2">
+        <v>41000</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>1008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2">
+        <v>48000</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>1009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="2">
+        <v>42000</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="2">
-        <v>45000</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="2">
-        <v>36000</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="2">
-        <v>63000</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1004</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="2">
-        <v>47000</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1005</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="2">
-        <v>50000</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1006</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="2">
-        <v>65000</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1007</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="2">
-        <v>41000</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1008</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="2">
-        <v>48000</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1009</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="2">
-        <v>42000</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F3BB1-397D-4AFC-8E96-ABE0D0515A1B}">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
-  <dimension ref="A1:K10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="11" max="11" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1683,14 +1768,14 @@
       <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
-        <v>82</v>
+      <c r="J1" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="K1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1718,8 +1803,12 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" t="str">
+        <f>IF(E2:E10="Male","M","F")</f>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1747,8 +1836,12 @@
       <c r="I3" s="1">
         <v>42287</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">IF(E3:E11="Male","M","F")</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1776,8 +1869,12 @@
       <c r="I4" s="1">
         <v>42986</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1805,8 +1902,12 @@
       <c r="I5" s="1">
         <v>42341</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1834,8 +1935,12 @@
       <c r="I6" s="1">
         <v>42977</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1863,8 +1968,12 @@
       <c r="I7" s="1">
         <v>41528</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1892,8 +2001,12 @@
       <c r="I8" s="1">
         <v>41551</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1921,8 +2034,12 @@
       <c r="I9" s="1">
         <v>42116</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1949,6 +2066,10 @@
       </c>
       <c r="I10" s="1">
         <v>40800</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>M</v>
       </c>
     </row>
   </sheetData>
@@ -1957,22 +2078,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577B4A2A-B2F2-4EC9-9616-29355E7995DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="L1" sqref="L1:S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2000,14 +2121,21 @@
       <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -2035,8 +2163,12 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <f>LEN(B2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -2064,8 +2196,12 @@
       <c r="I3" s="1">
         <v>42287</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <f t="shared" ref="J3:J10" si="0">LEN(B3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -2093,8 +2229,12 @@
       <c r="I4" s="1">
         <v>42986</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -2122,8 +2262,12 @@
       <c r="I5" s="1">
         <v>42341</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -2151,8 +2295,12 @@
       <c r="I6" s="1">
         <v>42977</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -2180,8 +2328,12 @@
       <c r="I7" s="1">
         <v>41528</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -2209,8 +2361,12 @@
       <c r="I8" s="1">
         <v>41551</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -2238,8 +2394,12 @@
       <c r="I9" s="1">
         <v>42116</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -2266,6 +2426,10 @@
       </c>
       <c r="I10" s="1">
         <v>40800</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2274,23 +2438,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC954FE-DA24-43B2-AD9D-17E8CC017065}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="L2" sqref="L2:L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="10" max="10" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2322,16 +2486,16 @@
         <v>38</v>
       </c>
       <c r="K1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -2362,8 +2526,16 @@
       <c r="J2" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K2" t="str">
+        <f>LEFT(C2,3)</f>
+        <v>Hal</v>
+      </c>
+      <c r="L2" t="str">
+        <f>RIGHT(C2,3)</f>
+        <v>ert</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -2394,8 +2566,16 @@
       <c r="J3" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K10" si="0">LEFT(C3,3)</f>
+        <v>Bea</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L10" si="1">RIGHT(C3,3)</f>
+        <v>ley</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -2426,8 +2606,16 @@
       <c r="J4" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>Sch</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="1"/>
+        <v>ute</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -2458,8 +2646,16 @@
       <c r="J5" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>Mar</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>tin</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -2490,8 +2686,16 @@
       <c r="J6" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>Fle</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>son</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -2522,8 +2726,16 @@
       <c r="J7" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>Sco</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="1"/>
+        <v>ott</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -2554,8 +2766,16 @@
       <c r="J8" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>Pal</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="1"/>
+        <v>mer</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -2586,8 +2806,16 @@
       <c r="J9" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>Hud</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
+        <v>son</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -2617,6 +2845,14 @@
       </c>
       <c r="J10" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>Mal</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
+        <v>one</v>
       </c>
     </row>
   </sheetData>
@@ -2625,7 +2861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C4862C-FF60-4E24-9054-4C595B8DA66E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -2635,13 +2871,13 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2673,7 +2909,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -2703,7 +2939,7 @@
       </c>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -2733,7 +2969,7 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -2763,7 +2999,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -2793,7 +3029,7 @@
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -2823,7 +3059,7 @@
       </c>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -2853,7 +3089,7 @@
       </c>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -2883,7 +3119,7 @@
       </c>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -2913,7 +3149,7 @@
       </c>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -2943,10 +3179,10 @@
       </c>
       <c r="K10" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="H13" s="3"/>
     </row>
   </sheetData>
@@ -2955,23 +3191,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F69BBA-836F-48E1-B067-27B71B706556}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2999,14 +3235,16 @@
       <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -3034,8 +3272,12 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" t="str">
+        <f>TRIM(C2)</f>
+        <v>Halpert</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -3063,8 +3305,12 @@
       <c r="I3" s="1">
         <v>42287</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">TRIM(C3)</f>
+        <v>Beasley</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -3092,8 +3338,12 @@
       <c r="I4" s="1">
         <v>42986</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Schrute</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -3121,8 +3371,12 @@
       <c r="I5" s="1">
         <v>42341</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Martin</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -3150,8 +3404,12 @@
       <c r="I6" s="1">
         <v>42977</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Flenderson</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -3179,8 +3437,12 @@
       <c r="I7" s="1">
         <v>41528</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Scott</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -3208,8 +3470,12 @@
       <c r="I8" s="1">
         <v>41551</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Palmer</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -3237,8 +3503,12 @@
       <c r="I9" s="1">
         <v>42116</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Hudson</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -3265,6 +3535,10 @@
       </c>
       <c r="I10" s="1">
         <v>40800</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Malone</v>
       </c>
     </row>
   </sheetData>
@@ -3273,24 +3547,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B9C42-087D-43BC-95CC-49AE54CDC17A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J1" sqref="J1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3318,17 +3592,18 @@
       <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -3356,8 +3631,12 @@
       <c r="I2" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J2" s="4" t="str">
+        <f>SUBSTITUTE(I2,"/","-")</f>
+        <v>9-6-2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -3385,8 +3664,12 @@
       <c r="I3" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J3" s="4" t="str">
+        <f t="shared" ref="J3:J10" si="0">SUBSTITUTE(I3,"/","-")</f>
+        <v>10-10-2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -3414,8 +3697,12 @@
       <c r="I4" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>9-8-2017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -3443,8 +3730,12 @@
       <c r="I5" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>12-3-2015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -3472,8 +3763,12 @@
       <c r="I6" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>8-30-2017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -3501,8 +3796,12 @@
       <c r="I7" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>9-11-2013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -3530,8 +3829,12 @@
       <c r="I8" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>9-11-2013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -3559,8 +3862,12 @@
       <c r="I9" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>4-22-2015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -3588,40 +3895,44 @@
       <c r="I10" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>4-22-2015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9">
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9">
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9">
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
@@ -3632,19 +3943,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D41C5D0-EC67-4288-8B29-30C6E5CFEE73}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3672,17 +3983,17 @@
       <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="28.8">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -3710,8 +4021,20 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <f>SUM(G2:G10)</f>
+        <v>437000</v>
+      </c>
+      <c r="K2">
+        <f>SUMIF(G2:G10,"&gt;45000")</f>
+        <v>273000</v>
+      </c>
+      <c r="L2" s="5">
+        <f>SUMIFS(G2:G10,G2:G10,"&gt;45000",G2:G10,"&lt;50000")</f>
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -3740,7 +4063,7 @@
         <v>42287</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -3769,7 +4092,7 @@
         <v>42986</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -3798,7 +4121,7 @@
         <v>42341</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -3827,7 +4150,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -3856,7 +4179,7 @@
         <v>41528</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -3885,7 +4208,7 @@
         <v>41551</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -3914,7 +4237,7 @@
         <v>42116</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -3949,23 +4272,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D217F6E-9452-40AF-AFA2-377600A25F44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -4003,7 +4326,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -4031,8 +4354,16 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <f>COUNT(A2:A10)</f>
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(D2:D10,"&gt;30")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -4061,7 +4392,7 @@
         <v>42287</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -4090,7 +4421,7 @@
         <v>42986</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -4119,7 +4450,7 @@
         <v>42341</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -4148,7 +4479,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -4177,7 +4508,7 @@
         <v>41528</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -4206,7 +4537,7 @@
         <v>41551</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -4235,7 +4566,7 @@
         <v>42116</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>1009</v>
       </c>

</xml_diff>